<commit_message>
Added machine learning components
</commit_message>
<xml_diff>
--- a/Data Collection & Processes/Referee Data/Referee Info [Dataset]/Referee Data.xlsx
+++ b/Data Collection & Processes/Referee Data/Referee Info [Dataset]/Referee Data.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinmedina/code/finalproject/referee info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinmedina/code/finalproject/Data Collection &amp; Processes/Referee Data/Referee Info [Dataset]/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA3AC06-EB69-CF4E-B8D1-67497397B659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531844BA-AC17-A840-ACC4-19248DD22F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4940" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{B4B970EC-E54E-C743-B9F5-FF3F0C393208}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{B4B970EC-E54E-C743-B9F5-FF3F0C393208}"/>
   </bookViews>
   <sheets>
     <sheet name="Unique Refs" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Unique Refs'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Unique Refs'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="121">
   <si>
     <t>Referee</t>
   </si>
@@ -372,6 +372,36 @@
   </si>
   <si>
     <t>Major City</t>
+  </si>
+  <si>
+    <t>BirthCityNearestToPremierLeagueStadium</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Wolverhampton</t>
+  </si>
+  <si>
+    <t>Blackburn</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Midlands</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>RefereeBirthCity_ByRegion</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -394,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,6 +443,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -426,17 +462,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -766,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A061B52-6989-3D47-B2AA-9058BDCFB4EF}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,9 +839,12 @@
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -793,11 +857,23 @@
       <c r="D1" t="s">
         <v>110</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="I1" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -810,11 +886,25 @@
       <c r="D2" t="s">
         <v>97</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H2" s="6">
+        <f>G2*0.8</f>
+        <v>23.200000000000003</v>
+      </c>
+      <c r="I2" s="6">
+        <f>G2*0.2</f>
+        <v>5.8000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -827,11 +917,25 @@
       <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3">
         <v>333</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H3" s="6">
+        <f t="shared" ref="H3:H51" si="0">G3*0.8</f>
+        <v>266.40000000000003</v>
+      </c>
+      <c r="I3" s="6">
+        <f t="shared" ref="I3:I51" si="1">G3*0.2</f>
+        <v>66.600000000000009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -844,11 +948,25 @@
       <c r="D4" t="s">
         <v>100</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H4" s="6">
+        <f t="shared" si="0"/>
+        <v>31.200000000000003</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="shared" si="1"/>
+        <v>7.8000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -861,11 +979,25 @@
       <c r="D5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5">
         <v>271</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H5" s="6">
+        <f t="shared" si="0"/>
+        <v>216.8</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" si="1"/>
+        <v>54.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -878,11 +1010,25 @@
       <c r="D6" t="s">
         <v>84</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H6" s="6">
+        <f t="shared" si="0"/>
+        <v>152.80000000000001</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" si="1"/>
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -895,11 +1041,25 @@
       <c r="D7" t="s">
         <v>108</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7">
         <v>214</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H7" s="6">
+        <f t="shared" si="0"/>
+        <v>171.20000000000002</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="1"/>
+        <v>42.800000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -912,11 +1072,25 @@
       <c r="D8" t="s">
         <v>107</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8">
         <v>205</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H8" s="6">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -929,11 +1103,25 @@
       <c r="D9" t="s">
         <v>99</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>30.400000000000002</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>7.6000000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -946,11 +1134,25 @@
       <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H10" s="6">
+        <f t="shared" si="0"/>
+        <v>50.400000000000006</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="1"/>
+        <v>12.600000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -963,11 +1165,25 @@
       <c r="D11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11">
         <v>361</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>288.8</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -980,11 +1196,25 @@
       <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H12" s="6">
+        <f t="shared" si="0"/>
+        <v>90.4</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="1"/>
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -997,11 +1227,25 @@
       <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H13" s="6">
+        <f t="shared" si="0"/>
+        <v>74.400000000000006</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1014,11 +1258,25 @@
       <c r="D14" t="s">
         <v>65</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H14" s="6">
+        <f t="shared" si="0"/>
+        <v>48.800000000000004</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="1"/>
+        <v>12.200000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -1031,11 +1289,25 @@
       <c r="D15" t="s">
         <v>96</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H15" s="6">
+        <f t="shared" si="0"/>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="1"/>
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1048,11 +1320,25 @@
       <c r="D16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16">
         <v>369</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H16" s="6">
+        <f t="shared" si="0"/>
+        <v>295.2</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="1"/>
+        <v>73.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1065,11 +1351,25 @@
       <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17">
         <v>135</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H17" s="6">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1082,11 +1382,25 @@
       <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H18" s="6">
+        <f t="shared" si="0"/>
+        <v>73.600000000000009</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="1"/>
+        <v>18.400000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1099,11 +1413,25 @@
       <c r="D19" t="s">
         <v>101</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>49.6</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="1"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1116,11 +1444,25 @@
       <c r="D20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20">
         <v>401</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H20" s="6">
+        <f t="shared" si="0"/>
+        <v>320.8</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="1"/>
+        <v>80.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1133,11 +1475,25 @@
       <c r="D21" t="s">
         <v>60</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21">
         <v>248</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H21" s="6">
+        <f t="shared" si="0"/>
+        <v>198.4</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="1"/>
+        <v>49.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1150,11 +1506,25 @@
       <c r="D22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22">
         <v>183</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H22" s="6">
+        <f t="shared" si="0"/>
+        <v>146.4</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="1"/>
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1167,11 +1537,25 @@
       <c r="D23" t="s">
         <v>60</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23">
         <v>164</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H23" s="6">
+        <f t="shared" si="0"/>
+        <v>131.20000000000002</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="1"/>
+        <v>32.800000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1184,11 +1568,25 @@
       <c r="D24" t="s">
         <v>98</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H24" s="6">
+        <f t="shared" si="0"/>
+        <v>29.6</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="1"/>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -1201,11 +1599,25 @@
       <c r="D25" t="s">
         <v>105</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25">
         <v>157</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H25" s="6">
+        <f t="shared" si="0"/>
+        <v>125.60000000000001</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="1"/>
+        <v>31.400000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -1218,11 +1630,25 @@
       <c r="D26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26">
         <v>400</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H26" s="6">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1235,11 +1661,25 @@
       <c r="D27" t="s">
         <v>63</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27">
         <v>275</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H27" s="6">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="I27" s="6">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1252,11 +1692,25 @@
       <c r="D28" t="s">
         <v>102</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H28" s="6">
+        <f t="shared" si="0"/>
+        <v>55.2</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="1"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
@@ -1269,11 +1723,25 @@
       <c r="D29" t="s">
         <v>104</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H29" s="6">
+        <f t="shared" si="0"/>
+        <v>89.600000000000009</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="1"/>
+        <v>22.400000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1286,11 +1754,25 @@
       <c r="D30" t="s">
         <v>76</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30">
         <v>125</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H30" s="6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -1303,11 +1785,25 @@
       <c r="D31" t="s">
         <v>76</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31">
         <v>107</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H31" s="6">
+        <f t="shared" si="0"/>
+        <v>85.600000000000009</v>
+      </c>
+      <c r="I31" s="6">
+        <f t="shared" si="1"/>
+        <v>21.400000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -1320,11 +1816,25 @@
       <c r="D32" t="s">
         <v>83</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32">
         <v>133</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H32" s="6">
+        <f t="shared" si="0"/>
+        <v>106.4</v>
+      </c>
+      <c r="I32" s="6">
+        <f t="shared" si="1"/>
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>20</v>
       </c>
@@ -1337,11 +1847,25 @@
       <c r="D33" t="s">
         <v>83</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H33" s="6">
+        <f t="shared" si="0"/>
+        <v>74.400000000000006</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" si="1"/>
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
@@ -1354,11 +1878,25 @@
       <c r="D34" t="s">
         <v>83</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G34">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H34" s="6">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1371,11 +1909,25 @@
       <c r="D35" t="s">
         <v>83</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G35">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H35" s="6">
+        <f t="shared" si="0"/>
+        <v>18.400000000000002</v>
+      </c>
+      <c r="I35" s="6">
+        <f t="shared" si="1"/>
+        <v>4.6000000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>26</v>
       </c>
@@ -1388,11 +1940,25 @@
       <c r="D36" t="s">
         <v>103</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G36">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H36" s="6">
+        <f t="shared" si="0"/>
+        <v>73.600000000000009</v>
+      </c>
+      <c r="I36" s="6">
+        <f t="shared" si="1"/>
+        <v>18.400000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
@@ -1405,11 +1971,25 @@
       <c r="D37" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37">
         <v>268</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H37" s="6">
+        <f t="shared" si="0"/>
+        <v>214.4</v>
+      </c>
+      <c r="I37" s="6">
+        <f t="shared" si="1"/>
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>35</v>
       </c>
@@ -1422,11 +2002,25 @@
       <c r="D38" t="s">
         <v>56</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G38">
         <v>146</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H38" s="6">
+        <f t="shared" si="0"/>
+        <v>116.80000000000001</v>
+      </c>
+      <c r="I38" s="6">
+        <f t="shared" si="1"/>
+        <v>29.200000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -1439,11 +2033,25 @@
       <c r="D39" t="s">
         <v>56</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G39">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H39" s="6">
+        <f t="shared" si="0"/>
+        <v>61.6</v>
+      </c>
+      <c r="I39" s="6">
+        <f t="shared" si="1"/>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1456,11 +2064,25 @@
       <c r="D40" t="s">
         <v>56</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G40">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H40" s="6">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="I40" s="6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>34</v>
       </c>
@@ -1473,11 +2095,25 @@
       <c r="D41" t="s">
         <v>106</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G41">
         <v>162</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H41" s="6">
+        <f t="shared" si="0"/>
+        <v>129.6</v>
+      </c>
+      <c r="I41" s="6">
+        <f t="shared" si="1"/>
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1490,11 +2126,22 @@
       <c r="D42" t="s">
         <v>80</v>
       </c>
-      <c r="E42">
+      <c r="F42" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H42" s="6">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="I42" s="6">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -1507,11 +2154,22 @@
       <c r="D43" t="s">
         <v>80</v>
       </c>
-      <c r="E43">
+      <c r="F43" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H43" s="6">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+      <c r="I43" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -1524,11 +2182,22 @@
       <c r="D44" t="s">
         <v>80</v>
       </c>
-      <c r="E44">
+      <c r="F44" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H44" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I44" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>32</v>
       </c>
@@ -1541,11 +2210,22 @@
       <c r="D45" t="s">
         <v>80</v>
       </c>
-      <c r="E45">
+      <c r="F45" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H45" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="I45" s="6">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
@@ -1558,11 +2238,22 @@
       <c r="D46" t="s">
         <v>80</v>
       </c>
-      <c r="E46">
+      <c r="F46" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H46" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="I46" s="6">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1575,11 +2266,22 @@
       <c r="D47" t="s">
         <v>80</v>
       </c>
-      <c r="E47">
+      <c r="F47" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H47" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="I47" s="6">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -1592,11 +2294,22 @@
       <c r="D48" t="s">
         <v>80</v>
       </c>
-      <c r="E48">
+      <c r="F48" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H48" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="I48" s="6">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -1609,11 +2322,22 @@
       <c r="D49" t="s">
         <v>80</v>
       </c>
-      <c r="E49">
+      <c r="F49" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H49" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="I49" s="6">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1626,11 +2350,22 @@
       <c r="D50" t="s">
         <v>80</v>
       </c>
-      <c r="E50">
+      <c r="F50" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H50" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="I50" s="6">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>25</v>
       </c>
@@ -1643,13 +2378,24 @@
       <c r="D51" t="s">
         <v>80</v>
       </c>
-      <c r="E51">
+      <c r="F51" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G51">
         <v>1</v>
       </c>
+      <c r="H51" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="I51" s="6">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{6A061B52-6989-3D47-B2AA-9058BDCFB4EF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
+  <autoFilter ref="A1:G1" xr:uid="{6A061B52-6989-3D47-B2AA-9058BDCFB4EF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G51">
       <sortCondition ref="D1:D51"/>
     </sortState>
   </autoFilter>

</xml_diff>